<commit_message>
sample .xlsx are added
</commit_message>
<xml_diff>
--- a/Leaderboards/01.xlsx
+++ b/Leaderboards/01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CSE LAB\Desktop\lab\Vjudge_Rank_System\Ranking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maruf\vs_file\Team_Formation_From_Vjudge_Standings\Leaderboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC34EF3-F471-44B9-BEE1-45A49F2118E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="99">
   <si>
     <t>Rank</t>
   </si>
@@ -355,12 +356,15 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a sample exported input.xlsx of a vjudge contest. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -391,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,16 +734,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -803,7 +807,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -835,7 +839,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -867,7 +871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -899,7 +903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -931,7 +935,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -963,7 +967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -995,7 +999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1027,7 +1031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -1059,7 +1063,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>63</v>
       </c>
@@ -1091,7 +1095,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1123,7 +1127,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -1155,7 +1159,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -1187,7 +1191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -1219,7 +1223,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -1251,7 +1255,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -1283,24 +1287,29 @@
         <v>16</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B7" r:id="rId6"/>
-    <hyperlink ref="B8" r:id="rId7"/>
-    <hyperlink ref="B9" r:id="rId8"/>
-    <hyperlink ref="B10" r:id="rId9"/>
-    <hyperlink ref="B11" r:id="rId10"/>
-    <hyperlink ref="B12" r:id="rId11"/>
-    <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
-    <hyperlink ref="B16" r:id="rId15"/>
-    <hyperlink ref="B17" r:id="rId16"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>